<commit_message>
Revert "Merge pull request #1 from zmcgrath96/working"
This reverts commit 5795d2512e57a1cce3ed212e1f30db8248cc521f, reversing
changes made to 64751b60558be42ac235ba6731b61fa4bf883684.
</commit_message>
<xml_diff>
--- a/Documentation/Scrum Artifacts/Meeting Log.xlsx
+++ b/Documentation/Scrum Artifacts/Meeting Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach\Documents\GitHub\Project4\Documentation\Scrum Artifacts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach\Documents\GitHub\Project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Day</t>
   </si>
@@ -162,42 +162,6 @@
   </si>
   <si>
     <t>Start merging map anc characters</t>
-  </si>
-  <si>
-    <t>Talked about new features</t>
-  </si>
-  <si>
-    <t>Start working on new features/add animations</t>
-  </si>
-  <si>
-    <t>Added animations and started on level progression</t>
-  </si>
-  <si>
-    <t>Finish Level Generation</t>
-  </si>
-  <si>
-    <t>Finished Level Progression</t>
-  </si>
-  <si>
-    <t>Add Item Interaction</t>
-  </si>
-  <si>
-    <t>3:00-4:30 pm</t>
-  </si>
-  <si>
-    <t>Finished item interaction and started pause menu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00 - 10:00 am </t>
-  </si>
-  <si>
-    <t>Pause Menu finished, add music</t>
-  </si>
-  <si>
-    <t>Finished pause menu and made progress on music</t>
-  </si>
-  <si>
-    <t>Finish with music and implement new players</t>
   </si>
 </sst>
 </file>
@@ -300,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,9 +336,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -665,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -676,7 +637,7 @@
     <col min="1" max="1" width="14.453125" customWidth="1"/>
     <col min="2" max="2" width="22.81640625" customWidth="1"/>
     <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="47.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.36328125" customWidth="1"/>
   </cols>
@@ -964,122 +925,52 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="25">
-        <v>43201</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="25">
-        <v>43201</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="25">
-        <v>43206</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="25">
-        <v>43208</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="25">
-        <v>43213</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
@@ -1705,14 +1596,6 @@
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>